<commit_message>
Fix typos in main block assignments
</commit_message>
<xml_diff>
--- a/html/resources/1condition/blockOrderA.xlsx
+++ b/html/resources/1condition/blockOrderA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janet/Documents/Sinai_Projects/Code/fish-task-6B20T/html/resources/1condition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9529AAE-3F59-B34C-9FA5-F57FF1F3D1AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D02D33-F683-F148-BD72-202781B7957C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="13980" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24700" yWindow="500" windowWidth="13980" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,30 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>condsFile</t>
   </si>
   <si>
     <t>readyMsg</t>
-  </si>
-  <si>
-    <t>C1 B1- 12,8: (213),(231)</t>
-  </si>
-  <si>
-    <t>C2 B2- 10,10: (123),(312)</t>
-  </si>
-  <si>
-    <t>C3 B3- 13,7: (321),(132)</t>
-  </si>
-  <si>
-    <t>C4 B4- 7,7,6: (231),(213),(132)</t>
-  </si>
-  <si>
-    <t>C5 B5- 8,12: (132),(321)</t>
-  </si>
-  <si>
-    <t>C6 B6- 7,13: (312),(123)</t>
   </si>
   <si>
     <t>1condition/mainTrials1.xlsx</t>
@@ -403,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -427,70 +409,52 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>